<commit_message>
initial attempt at shr linkage, cleanup of github instructions, and preview of special case articles
</commit_message>
<xml_diff>
--- a/orphan_matches_final.xlsx
+++ b/orphan_matches_final.xlsx
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="X16" t="n">
-        <v>0.995695069691549</v>
+        <v>0.9985998639519477</v>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="X18" t="n">
-        <v>0.9734555597192146</v>
+        <v>0.974017887484168</v>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
@@ -2989,7 +2989,7 @@
         </is>
       </c>
       <c r="X32" t="n">
-        <v>0.9998187602249933</v>
+        <v>0.9998227013982782</v>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
@@ -3560,7 +3560,7 @@
         </is>
       </c>
       <c r="X39" t="n">
-        <v>0.9999999290812993</v>
+        <v>0.9999999285564317</v>
       </c>
       <c r="Y39" t="inlineStr">
         <is>
@@ -3727,7 +3727,7 @@
         </is>
       </c>
       <c r="X41" t="n">
-        <v>0.9999963557622197</v>
+        <v>0.9999964276956776</v>
       </c>
       <c r="Y41" t="inlineStr">
         <is>
@@ -5807,7 +5807,7 @@
         </is>
       </c>
       <c r="X67" t="n">
-        <v>0.4894330181186596</v>
+        <v>0.6434744741786268</v>
       </c>
       <c r="Y67" t="inlineStr">
         <is>
@@ -5874,7 +5874,7 @@
         </is>
       </c>
       <c r="X68" t="n">
-        <v>0.2809124097104978</v>
+        <v>0.3284075266776713</v>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
@@ -5935,7 +5935,7 @@
         </is>
       </c>
       <c r="X69" t="n">
-        <v>0.4007900319920537</v>
+        <v>0.6260908230868526</v>
       </c>
       <c r="Y69" t="inlineStr">
         <is>
@@ -5996,7 +5996,7 @@
         </is>
       </c>
       <c r="X70" t="n">
-        <v>0.6809244403278467</v>
+        <v>0.842331686272997</v>
       </c>
       <c r="Y70" t="inlineStr">
         <is>

</xml_diff>